<commit_message>
Updated DEU_grids model - 2025-09-06 13:38
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/SuppXLS/trades/scentrade__trade_links.xlsx
+++ b/VerveStacks_DEU_grids/SuppXLS/trades/scentrade__trade_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\SuppXLS\trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25672820-B5D7-4432-8749-F6D25B0F3893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E7B7E29-64AB-47A5-ABF9-040ABC273300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{A4B3E96B-1BE2-4619-8CB2-DD6BFCE59B59}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{CC1AFB81-D103-49ED-A5CE-23F23BBB7E18}"/>
   </bookViews>
   <sheets>
     <sheet name="grid_links" sheetId="1" r:id="rId1"/>
@@ -6019,7 +6019,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4EFE7A-B1A8-4B18-9367-06298492D6FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE30F38F-C5EE-493E-AD78-BC2E34234942}">
   <dimension ref="B3:L896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>